<commit_message>
config change ,delete email value from orchestator sheet
</commit_message>
<xml_diff>
--- a/configulation.xlsx
+++ b/configulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BARA\Documents\UiPath\HMC_Control_Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B7EF98-F3D1-41A2-B982-E29791C11157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A386F6-4566-4DEA-BD02-6AE9988F81EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ORCHESTRATOR_VARIABLE" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>Value</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>strEmailList</t>
   </si>
   <si>
     <t>Asset</t>
@@ -670,9 +667,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -689,40 +686,34 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B3" s="7"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="B4" s="7"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="B5" s="7"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -745,15 +736,10 @@
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -789,73 +775,73 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>43</v>
       </c>
       <c r="C2" s="17"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>44</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="17"/>
     </row>
     <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="17"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="17"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="17"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="17"/>
     </row>
@@ -875,7 +861,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A14" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,116 +884,116 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="15"/>
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>25</v>
       </c>
       <c r="C11" s="17"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="C14" s="17"/>
     </row>
@@ -1025,7 +1011,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,7 +1034,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="18">
         <v>0</v>
@@ -1057,7 +1043,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="18">
         <v>5</v>
@@ -1066,73 +1052,73 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="17"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>20</v>
       </c>
       <c r="C5" s="17"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="17"/>
     </row>
     <row r="7" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="C7" s="17"/>
     </row>
     <row r="8" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>54</v>
       </c>
       <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="17"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="17"/>
     </row>
@@ -1150,7 +1136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1163,35 +1149,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IF object not set to instance
</commit_message>
<xml_diff>
--- a/configulation.xlsx
+++ b/configulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BARA\Documents\UiPath\HMC_Control_Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Departments\Technology\QA\RPA2022\NONPRODUCTION\CONTROLCHART\UIpathProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96128CBC-8134-40B6-91ED-127F0C867E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7F6DD9-4E05-493D-9CD4-67F506FDD300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,9 +221,6 @@
     <t>Non production/QA_Control_Chart</t>
   </si>
   <si>
-    <t>CRTL_ReportExecutionWeekly</t>
-  </si>
-  <si>
     <t>CTRL_strEmailQATeamList</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>LIMS_strBusinessErrorMailSubject</t>
+  </si>
+  <si>
+    <t>CTRL_ReportExecutionWeekly</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -754,7 +754,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>58</v>
@@ -765,7 +765,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>58</v>
@@ -776,7 +776,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>58</v>
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>58</v>
@@ -798,7 +798,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>58</v>
@@ -809,7 +809,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>58</v>
@@ -820,7 +820,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>58</v>
@@ -831,7 +831,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>58</v>
@@ -842,7 +842,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>58</v>
@@ -853,7 +853,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>58</v>
@@ -864,7 +864,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>58</v>
@@ -875,7 +875,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>58</v>
@@ -886,7 +886,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>58</v>
@@ -897,7 +897,7 @@
         <v>25</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>58</v>
@@ -905,10 +905,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>58</v>
@@ -919,7 +919,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>58</v>
@@ -930,7 +930,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>58</v>
@@ -941,7 +941,7 @@
         <v>30</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>58</v>
@@ -952,7 +952,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>58</v>
@@ -960,10 +960,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>58</v>
@@ -974,7 +974,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>58</v>
@@ -1022,7 +1022,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>58</v>
@@ -1177,7 +1177,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="16"/>
     </row>

</xml_diff>

<commit_message>
use strNoAbnormalWeeklyReport at config
</commit_message>
<xml_diff>
--- a/configulation.xlsx
+++ b/configulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Departments\Technology\QA\RPA2022\NONPRODUCTION\CONTROLCHART\UIpathProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF608271-1080-487B-A299-7028F77B3AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E53692-5139-493C-9B51-7544878BD703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>Value</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>14/09/2021</t>
+  </si>
+  <si>
+    <t>strNoAbnormalWeeklyReport</t>
+  </si>
+  <si>
+    <t>The Last week's Lims Control Chart Data do not have any Abnormal Events.</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,6 +1250,15 @@
         <v>58</v>
       </c>
       <c r="C15" s="16"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="16"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C23">

</xml_diff>